<commit_message>
negative scenario and excel sheet, cess amount updated
negative scenario feature file created, excel sheet, cess amount updated
</commit_message>
<xml_diff>
--- a/testdata/sample inventory all.xlsx
+++ b/testdata/sample inventory all.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="137">
   <si>
     <t xml:space="preserve">PriceType</t>
   </si>
@@ -50,6 +50,12 @@
     <t xml:space="preserve">GSTPer</t>
   </si>
   <si>
+    <t xml:space="preserve">Cess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AdlCsAmt</t>
+  </si>
+  <si>
     <t xml:space="preserve">NetSellingPrice</t>
   </si>
   <si>
@@ -59,6 +65,15 @@
     <t xml:space="preserve">netcost</t>
   </si>
   <si>
+    <t xml:space="preserve">WPrice1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WPrice2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WPrice3</t>
+  </si>
+  <si>
     <t xml:space="preserve">InventoryType</t>
   </si>
   <si>
@@ -290,75 +305,72 @@
     <t xml:space="preserve">cost4</t>
   </si>
   <si>
+    <t xml:space="preserve">110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MRP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">97.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91.46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">128.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">198</t>
+  </si>
+  <si>
+    <t xml:space="preserve">211.86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">116.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MRP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75.60</t>
+  </si>
+  <si>
     <t xml:space="preserve">500</t>
   </si>
   <si>
-    <t xml:space="preserve">350</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">436.58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">250</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">236</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MRP1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">97.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">98</t>
-  </si>
-  <si>
-    <t xml:space="preserve">91.46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">128.58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">198</t>
-  </si>
-  <si>
-    <t xml:space="preserve">211.86</t>
-  </si>
-  <si>
-    <t xml:space="preserve">150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">116.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MRP2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75.60</t>
-  </si>
-  <si>
     <t xml:space="preserve">462</t>
   </si>
   <si>
@@ -411,6 +423,9 @@
   </si>
   <si>
     <t xml:space="preserve">MRP5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5</t>
   </si>
   <si>
     <t xml:space="preserve">33.95</t>
@@ -588,27 +603,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AS24"/>
+  <dimension ref="A1:AX24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R5" activeCellId="0" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="19.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.0663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="40.6938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="36.6479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.9285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.8877551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="22.8877551020408"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="39.6887755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="30.4744897959184"/>
-    <col collapsed="false" hidden="false" max="22" min="12" style="0" width="18.3214285714286"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="18.3214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="22.8877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="48.3877551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="43.5408163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="31.8928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="32.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.7295918367347"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.7551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="46.9795918367347"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="36.2397959183673"/>
+    <col collapsed="false" hidden="false" max="27" min="14" style="0" width="21.5612244897959"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="25.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="21.5612244897959"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -645,22 +662,22 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="0" t="s">
@@ -747,52 +764,61 @@
       <c r="AS1" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="AT1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="0" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="0" t="n">
         <v>47.05</v>
       </c>
-      <c r="M2" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>58</v>
+      <c r="O2" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>1.8</v>
       </c>
       <c r="R2" s="0" t="s">
         <v>59</v>
@@ -801,28 +827,28 @@
         <v>60</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="V2" s="5" t="n">
+        <v>62</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA2" s="5" t="n">
         <v>1</v>
-      </c>
-      <c r="W2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z2" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>66</v>
       </c>
       <c r="AB2" s="0" t="s">
         <v>67</v>
@@ -830,171 +856,228 @@
       <c r="AC2" s="0" t="s">
         <v>68</v>
       </c>
+      <c r="AD2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>70</v>
+      </c>
       <c r="AF2" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AG2" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="AH2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI2" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ2" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="AK2" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM2" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AO2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="AL2" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="AM2" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="AN2" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="AO2" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="AP2" s="0" t="n">
+      <c r="AQ2" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="AS2" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU2" s="0" t="n">
         <v>12.456</v>
       </c>
-      <c r="AQ2" s="0" t="n">
+      <c r="AV2" s="0" t="n">
         <v>2.5</v>
       </c>
-      <c r="AR2" s="0" t="n">
+      <c r="AW2" s="0" t="n">
         <v>122.5</v>
       </c>
-      <c r="AS2" s="0" t="n">
+      <c r="AX2" s="0" t="n">
         <v>323.4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L3" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="0" t="n">
         <v>47.98</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J4" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" s="0" t="n">
+      <c r="L4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N4" s="0" t="n">
         <v>448</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L5" s="0" t="n">
-        <v>363.82</v>
+        <v>95</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="X5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z5" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC5" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD5" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE5" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF5" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG5" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH5" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L6" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N6" s="0" t="n">
         <v>236</v>
       </c>
     </row>
@@ -1016,146 +1099,211 @@
       <c r="I7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" s="4" t="s">
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="M7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L8" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N8" s="0" t="n">
         <v>97.02</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="R8" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="T8" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="U8" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="V8" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="W8" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="X8" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y8" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z8" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC8" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD8" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE8" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF8" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG8" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH8" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L9" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N9" s="0" t="n">
         <v>96.04</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L10" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N10" s="0" t="n">
         <v>144</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L11" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N11" s="0" t="n">
         <v>250</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L12" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N12" s="0" t="n">
         <v>148.5</v>
       </c>
     </row>
@@ -1177,94 +1325,159 @@
       <c r="I13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L13" s="4" t="s">
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="M13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="L14" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N14" s="0" t="n">
         <v>72</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="R14" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="S14" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="T14" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="U14" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="V14" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="W14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="X14" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y14" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z14" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA14" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC14" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD14" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE14" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF14" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG14" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH14" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L15" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N15" s="0" t="n">
         <v>485.1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L16" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N16" s="0" t="n">
         <v>9.7</v>
       </c>
     </row>
@@ -1286,94 +1499,159 @@
       <c r="I17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L17" s="4" t="s">
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="M17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L18" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="N18" s="0" t="n">
         <v>9.8</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="P18" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="R18" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="S18" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="T18" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="U18" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="V18" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="W18" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="X18" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y18" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z18" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA18" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB18" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC18" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD18" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE18" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF18" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG18" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH18" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L19" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N19" s="0" t="n">
         <v>20.78</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="L20" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N20" s="0" t="n">
         <v>34.7</v>
       </c>
     </row>
@@ -1395,98 +1673,229 @@
       <c r="I21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L21" s="4" t="s">
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="M21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L22" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N22" s="0" t="n">
         <v>9.7</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="P22" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="Q22" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="R22" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="S22" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="T22" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="U22" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="V22" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="W22" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="X22" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y22" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z22" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA22" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB22" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC22" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD22" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE22" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF22" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG22" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH22" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="L23" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="N23" s="0" t="n">
         <v>20.38</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="L24" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="N24" s="0" t="n">
         <v>32.92</v>
+      </c>
+      <c r="O24" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="P24" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="Q24" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="R24" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="S24" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="T24" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="U24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="V24" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="W24" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="X24" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y24" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z24" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA24" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB24" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC24" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD24" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE24" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF24" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG24" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH24" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1513,7 +1922,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="18.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="21.5612244897959"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>